<commit_message>
commiting files of entity Change Request: Adding and removing files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/CR Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/CR Suite.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="ChangeRequestNonWorkflow" sheetId="7" r:id="rId2"/>
+    <sheet name="ChangeRequestUpdate" sheetId="7" r:id="rId2"/>
     <sheet name="ChangeRequestCreation" sheetId="5" r:id="rId3"/>
     <sheet name="ActionCreation" sheetId="2" r:id="rId4"/>
     <sheet name="InterpretationCreation" sheetId="3" r:id="rId5"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="178">
   <si>
     <t>TCID</t>
   </si>
@@ -396,88 +396,163 @@
     <t>ABC News</t>
   </si>
   <si>
+    <t>Master Service Agreement - ABC</t>
+  </si>
+  <si>
+    <t>Logo colour change</t>
+  </si>
+  <si>
+    <t>Logo should contain only blue and red colour.</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Modify Rate Card</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>crOriginalTCV</t>
+  </si>
+  <si>
+    <t>crCurrOriginalTCV</t>
+  </si>
+  <si>
+    <t>crRevisedTCV</t>
+  </si>
+  <si>
+    <t>crCurrRevisedTCV</t>
+  </si>
+  <si>
+    <t>crVarianceTCV</t>
+  </si>
+  <si>
+    <t>crCurrVarianceTCV</t>
+  </si>
+  <si>
+    <t>crVarianceACV</t>
+  </si>
+  <si>
+    <t>crCurrVarianceACV</t>
+  </si>
+  <si>
+    <t>Australian Dollar (AUD)</t>
+  </si>
+  <si>
+    <t>crOriginalFACV</t>
+  </si>
+  <si>
+    <t>crCurrOriginalFACV</t>
+  </si>
+  <si>
+    <t>crRevisedFACV</t>
+  </si>
+  <si>
+    <t>crCurrRevisedFACV</t>
+  </si>
+  <si>
+    <t>crVarianceFACV</t>
+  </si>
+  <si>
+    <t>crCurrVarianceFACV</t>
+  </si>
+  <si>
+    <t>ChangeRequestWorkflow</t>
+  </si>
+  <si>
+    <t>PerformingChangeRequestWorkflowSteps</t>
+  </si>
+  <si>
+    <t>Logo colour change edited</t>
+  </si>
+  <si>
+    <t>Logo should contain only blue and red colour edited.</t>
+  </si>
+  <si>
+    <t>Asia/Kathmandu (GMT +05:45)</t>
+  </si>
+  <si>
+    <t>Non-Contract</t>
+  </si>
+  <si>
+    <t>Modify Transition Plan</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Change Request Initiated</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Applications Development &amp; Maintenance , Applications Servers , LAN , Mainframe Services , Network MNS</t>
+  </si>
+  <si>
+    <t>APAC</t>
+  </si>
+  <si>
+    <t>Albania , Algeria , Rest of APAC , Afghanistan , Akrotiri , Angola , Anguilla , American Samoa , Andorra , Argentina , Armenia , Antarctica , Antigua and Barbuda , Australia , Austria , Aruba , Ashmore and Cartier Islands , Azerbaijan</t>
+  </si>
+  <si>
+    <t>crComment</t>
+  </si>
+  <si>
+    <t>Change request should not take more than 15 days</t>
+  </si>
+  <si>
+    <t>Change request should not take more than 15 days edited</t>
+  </si>
+  <si>
+    <t>Contracts</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CRListing</t>
+  </si>
+  <si>
+    <t>OpenCRFromListing</t>
+  </si>
+  <si>
+    <t>ActionCreation</t>
+  </si>
+  <si>
+    <t>ActionCreation description</t>
+  </si>
+  <si>
+    <t>IssueCreation</t>
+  </si>
+  <si>
+    <t>IssueCreation description</t>
+  </si>
+  <si>
+    <t>InterpretationCreation</t>
+  </si>
+  <si>
+    <t>InterpretationCreation description</t>
+  </si>
+  <si>
     <t>MSA</t>
   </si>
   <si>
-    <t>Master Service Agreement - ABC</t>
-  </si>
-  <si>
-    <t>Logo colour change</t>
-  </si>
-  <si>
-    <t>Logo should contain only blue and red colour.</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Modify Rate Card</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>crOriginalTCV</t>
-  </si>
-  <si>
-    <t>crCurrOriginalTCV</t>
-  </si>
-  <si>
-    <t>crRevisedTCV</t>
-  </si>
-  <si>
-    <t>crCurrRevisedTCV</t>
-  </si>
-  <si>
-    <t>crVarianceTCV</t>
-  </si>
-  <si>
-    <t>crCurrVarianceTCV</t>
-  </si>
-  <si>
-    <t>crVarianceACV</t>
-  </si>
-  <si>
-    <t>crCurrVarianceACV</t>
-  </si>
-  <si>
-    <t>Australian Dollar (AUD)</t>
-  </si>
-  <si>
-    <t>crOriginalFACV</t>
-  </si>
-  <si>
-    <t>crCurrOriginalFACV</t>
-  </si>
-  <si>
-    <t>crRevisedFACV</t>
-  </si>
-  <si>
-    <t>crCurrRevisedFACV</t>
-  </si>
-  <si>
-    <t>crVarianceFACV</t>
-  </si>
-  <si>
-    <t>crCurrVarianceFACV</t>
-  </si>
-  <si>
-    <t>ChangeRequestWorkflow</t>
-  </si>
-  <si>
-    <t>ChangeRequestNonWorkflow</t>
-  </si>
-  <si>
-    <t>PerformingChangeRequestWorkflowSteps</t>
-  </si>
-  <si>
-    <t>PerformingChangeRequestNonWorkflowSteps</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Logo colour change edited</t>
+    <t>Asia/Kolkata (GMT +05:30)</t>
+  </si>
+  <si>
+    <t>Tier - 1</t>
+  </si>
+  <si>
+    <t>ChangeRequestUpdate</t>
+  </si>
+  <si>
+    <t>ChangeRequestUpdate description</t>
   </si>
 </sst>
 </file>
@@ -585,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -600,6 +675,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,28 +1030,32 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>149</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -981,6 +1063,66 @@
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -989,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU4"/>
+  <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,13 +1158,13 @@
     <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="44" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="45" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -1078,22 +1220,22 @@
         <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>91</v>
@@ -1108,28 +1250,28 @@
         <v>94</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="AE1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>97</v>
@@ -1153,19 +1295,22 @@
         <v>123</v>
       </c>
       <c r="AR1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1211,12 +1356,13 @@
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1262,135 +1408,143 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
-      <c r="AT3" s="1" t="s">
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="16">
+        <v>2</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="9">
+      <c r="K4" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="M4" s="16">
         <v>1</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="N4" s="16">
+        <v>2</v>
+      </c>
+      <c r="O4" s="16">
+        <v>2015</v>
+      </c>
+      <c r="P4" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>3</v>
+      </c>
+      <c r="R4" s="16">
+        <v>2017</v>
+      </c>
+      <c r="S4" s="16">
         <v>7</v>
       </c>
-      <c r="M4" s="9">
-        <v>1</v>
-      </c>
-      <c r="N4" s="9">
-        <v>2</v>
-      </c>
-      <c r="O4" s="9">
-        <v>2017</v>
-      </c>
-      <c r="P4" s="9">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>1</v>
-      </c>
-      <c r="R4" s="9">
-        <v>2017</v>
-      </c>
-      <c r="S4" s="9">
+      <c r="T4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="U4" s="16">
+        <v>11</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="W4" s="16">
         <v>5</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="X4" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="U4" s="9">
+      <c r="Y4" s="16">
         <v>10</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="Z4" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="9">
-        <v>5</v>
-      </c>
-      <c r="X4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y4" s="9">
-        <v>10</v>
-      </c>
-      <c r="Z4" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="16">
+        <v>22</v>
+      </c>
+      <c r="AB4" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC4" s="16">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE4" s="16">
+        <v>11</v>
+      </c>
+      <c r="AF4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG4" s="16">
         <v>20</v>
       </c>
-      <c r="AB4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC4" s="9">
-        <v>30</v>
-      </c>
-      <c r="AD4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE4" s="9">
-        <v>10</v>
-      </c>
-      <c r="AF4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG4" s="9">
-        <v>20</v>
-      </c>
-      <c r="AH4" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI4" s="9">
-        <v>30</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="AK4" s="9" t="s">
+      <c r="AH4" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI4" s="16">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="AK4" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9" t="s">
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AQ4" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="AQ4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9" t="s">
+      <c r="AR4" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="AT4" s="9" t="s">
+      <c r="AU4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AU4" s="9"/>
+      <c r="AV4" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1399,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU4"/>
+  <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AS4" sqref="AS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,13 +1580,13 @@
     <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="44" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="45" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -1488,22 +1642,22 @@
         <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>91</v>
@@ -1518,28 +1672,28 @@
         <v>94</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="AE1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>97</v>
@@ -1563,19 +1717,22 @@
         <v>123</v>
       </c>
       <c r="AR1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1621,12 +1778,13 @@
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1672,138 +1830,157 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
-      <c r="AT3" s="1" t="s">
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:48" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="14">
         <v>1</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="14">
         <v>1</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="14">
         <v>2</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="14">
         <v>2017</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="14">
         <v>3</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="14">
         <v>1</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="14">
         <v>2017</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="14">
         <v>5</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="14">
         <v>10</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="V4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="W4" s="9">
+      <c r="W4" s="14">
         <v>5</v>
       </c>
-      <c r="X4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y4" s="9">
+      <c r="X4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y4" s="14">
         <v>10</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Z4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="14">
         <v>20</v>
       </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AB4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AC4" s="14">
         <v>30</v>
       </c>
-      <c r="AD4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE4" s="9">
+      <c r="AD4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE4" s="14">
         <v>10</v>
       </c>
-      <c r="AF4" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AG4" s="9">
+      <c r="AF4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG4" s="14">
         <v>20</v>
       </c>
-      <c r="AH4" s="9" t="s">
+      <c r="AH4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AI4" s="14">
         <v>30</v>
       </c>
-      <c r="AJ4" s="9" t="s">
+      <c r="AJ4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="AK4" s="9" t="s">
+      <c r="AK4" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9" t="s">
+      <c r="AL4" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AO4" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AP4" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AQ4" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="AQ4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="9" t="s">
+      <c r="AR4" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="AS4" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AT4" s="9" t="s">
+      <c r="AU4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AU4" s="9"/>
+      <c r="AV4" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
todo suite and all integrated files working 5 entities suite commit
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/CR Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/CR Suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="179">
   <si>
     <t>TCID</t>
   </si>
@@ -553,12 +553,16 @@
   </si>
   <si>
     <t>ChangeRequestUpdate description</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -985,15 +989,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1058,11 +1062,9 @@
         <v>177</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1139,29 +1141,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="18" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="23" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.7109375" style="13" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="45" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="13" max="15" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="16" max="18" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="19" max="23" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="13" width="20.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="31" max="45" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
@@ -1561,29 +1563,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="18" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="23" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.7109375" style="13" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="45" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="13" max="15" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="16" max="18" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="19" max="23" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="13" width="20.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="31" max="45" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
@@ -1994,19 +1996,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="27" width="24" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="9" max="11" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="13" max="15" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="16" max="27" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -2180,26 +2182,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2335,28 +2337,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="34.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="32.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>